<commit_message>
Fixed lat lon issue. added drop-down widget
Fixed lat lon issue. added drop-down widget
</commit_message>
<xml_diff>
--- a/Data/Well_Headers.xlsx
+++ b/Data/Well_Headers.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\D$\DataScience\PyGeo\t20-Dash_Well_Viz\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScience\PyGeo\t20-Dash_Well_Viz\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D347F5E-B769-45E2-864B-87572D4C6F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23955" windowHeight="11565"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -95,11 +104,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.0000000"/>
-    <numFmt numFmtId="170" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -135,13 +144,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -423,11 +432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +508,7 @@
         <v>8481148.0199999996</v>
       </c>
       <c r="D2" s="1">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="E2" s="1">
         <v>44</v>
@@ -508,8 +517,8 @@
         <v>16.8752</v>
       </c>
       <c r="G2" s="3">
-        <f>D2+(E2/60)+(F2/3600)</f>
-        <v>13.738020888888888</v>
+        <f>D2-(E2/60)-(F2/3600)</f>
+        <v>-13.738020888888888</v>
       </c>
       <c r="H2" s="1">
         <v>122</v>
@@ -545,7 +554,7 @@
         <v>8485490.7300000004</v>
       </c>
       <c r="D3" s="1">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="E3" s="1">
         <v>41</v>
@@ -554,8 +563,8 @@
         <v>53.980200000000004</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G9" si="0">D3+(E3/60)+(F3/3600)</f>
-        <v>13.698327833333334</v>
+        <f t="shared" ref="G3:G9" si="0">D3-(E3/60)-(F3/3600)</f>
+        <v>-13.698327833333334</v>
       </c>
       <c r="H3" s="1">
         <v>122</v>
@@ -591,7 +600,7 @@
         <v>8490107.5199999996</v>
       </c>
       <c r="D4" s="1">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="E4" s="1">
         <v>39</v>
@@ -601,7 +610,7 @@
       </c>
       <c r="G4" s="3">
         <f t="shared" si="0"/>
-        <v>13.656908805555556</v>
+        <v>-13.656908805555556</v>
       </c>
       <c r="H4" s="1">
         <v>122</v>
@@ -637,7 +646,7 @@
         <v>8493875.2599999998</v>
       </c>
       <c r="D5" s="1">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="E5" s="1">
         <v>37</v>
@@ -647,7 +656,7 @@
       </c>
       <c r="G5" s="3">
         <f t="shared" si="0"/>
-        <v>13.622867833333334</v>
+        <v>-13.622867833333334</v>
       </c>
       <c r="H5" s="1">
         <v>122</v>
@@ -683,7 +692,7 @@
         <v>8487361.3900000006</v>
       </c>
       <c r="D6" s="1">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="E6" s="1">
         <v>40</v>
@@ -693,7 +702,7 @@
       </c>
       <c r="G6" s="3">
         <f t="shared" si="0"/>
-        <v>13.682004027777777</v>
+        <v>-13.682004027777777</v>
       </c>
       <c r="H6" s="1">
         <v>122</v>
@@ -729,7 +738,7 @@
         <v>8488800.7699999996</v>
       </c>
       <c r="D7" s="1">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="E7" s="1">
         <v>40</v>
@@ -739,7 +748,7 @@
       </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>13.668659666666667</v>
+        <v>-13.668659666666667</v>
       </c>
       <c r="H7" s="1">
         <v>122</v>
@@ -775,7 +784,7 @@
         <v>8499338.2699999996</v>
       </c>
       <c r="D8" s="1">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="E8" s="1">
         <v>34</v>
@@ -785,7 +794,7 @@
       </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>13.573562472222221</v>
+        <v>-13.573562472222221</v>
       </c>
       <c r="H8" s="1">
         <v>122</v>
@@ -821,7 +830,7 @@
         <v>8466761.5999999996</v>
       </c>
       <c r="D9" s="1">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="E9" s="1">
         <v>52</v>
@@ -831,7 +840,7 @@
       </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>13.867229555555555</v>
+        <v>-13.867229555555555</v>
       </c>
       <c r="H9" s="1">
         <v>122</v>

</xml_diff>